<commit_message>
PM test 5 contains digital input for frequency measurement
</commit_message>
<xml_diff>
--- a/LJDAQChannelGuide.xlsx
+++ b/LJDAQChannelGuide.xlsx
@@ -8,7 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Labjack Table" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621" concurrentCalc="0"/>
@@ -130,9 +130,6 @@
     <t>Sensor is open collector circuit, no supply voltage is needed.</t>
   </si>
   <si>
-    <t>Digital + Single (as of now)</t>
-  </si>
-  <si>
     <t>T coolant motor inlet</t>
   </si>
   <si>
@@ -296,6 +293,9 @@
   <si>
     <t xml:space="preserve">Positive:
 Negative: </t>
+  </si>
+  <si>
+    <t>Digital + Single</t>
   </si>
 </sst>
 </file>
@@ -430,7 +430,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -459,22 +459,33 @@
     <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -777,10 +788,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P29"/>
+  <dimension ref="A1:H29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C19" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2:P27"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -789,7 +800,7 @@
     <col min="2" max="8" width="22.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -815,7 +826,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" ht="39" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -832,17 +843,14 @@
         <v>11</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G2" s="3"/>
       <c r="H2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="L2" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:8" ht="39" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -859,29 +867,14 @@
         <v>16</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G3" s="3"/>
       <c r="H3" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="L3" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="M3" s="10" t="s">
-        <v>81</v>
-      </c>
-      <c r="N3" s="10" t="s">
-        <v>86</v>
-      </c>
-      <c r="O3" s="10" t="s">
-        <v>87</v>
-      </c>
-      <c r="P3" s="10" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:8" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -898,35 +891,14 @@
         <v>21</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G4" s="3"/>
       <c r="H4" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="J4" s="11" t="s">
-        <v>84</v>
-      </c>
-      <c r="K4" s="12">
-        <v>0</v>
-      </c>
-      <c r="L4">
-        <v>0</v>
-      </c>
-      <c r="M4">
-        <v>0</v>
-      </c>
-      <c r="N4">
-        <v>48</v>
-      </c>
-      <c r="O4">
-        <v>72</v>
-      </c>
-      <c r="P4">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:8" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -943,33 +915,14 @@
         <v>21</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G5" s="3"/>
       <c r="H5" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="J5" s="13"/>
-      <c r="K5" s="12">
-        <v>1</v>
-      </c>
-      <c r="L5">
-        <v>1</v>
-      </c>
-      <c r="M5">
-        <v>1</v>
-      </c>
-      <c r="N5">
-        <v>49</v>
-      </c>
-      <c r="O5">
-        <v>73</v>
-      </c>
-      <c r="P5">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:8" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -986,33 +939,14 @@
         <v>21</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G6" s="3"/>
       <c r="H6" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="J6" s="13"/>
-      <c r="K6" s="12">
-        <v>2</v>
-      </c>
-      <c r="L6">
-        <v>2</v>
-      </c>
-      <c r="M6">
-        <v>2</v>
-      </c>
-      <c r="N6">
-        <v>50</v>
-      </c>
-      <c r="O6">
-        <v>74</v>
-      </c>
-      <c r="P6">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:8" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -1029,33 +963,14 @@
         <v>21</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G7" s="3"/>
       <c r="H7" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="J7" s="13"/>
-      <c r="K7" s="12">
-        <v>3</v>
-      </c>
-      <c r="L7">
-        <v>3</v>
-      </c>
-      <c r="M7">
-        <v>3</v>
-      </c>
-      <c r="N7">
-        <v>51</v>
-      </c>
-      <c r="O7">
-        <v>75</v>
-      </c>
-      <c r="P7">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:8" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -1072,33 +987,14 @@
         <v>21</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G8" s="3"/>
       <c r="H8" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="J8" s="13"/>
-      <c r="K8" s="12">
-        <v>4</v>
-      </c>
-      <c r="L8" t="s">
-        <v>83</v>
-      </c>
-      <c r="M8">
-        <v>120</v>
-      </c>
-      <c r="N8">
-        <v>52</v>
-      </c>
-      <c r="O8">
-        <v>76</v>
-      </c>
-      <c r="P8">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:8" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -1115,33 +1011,14 @@
         <v>21</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G9" s="3"/>
       <c r="H9" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="J9" s="13"/>
-      <c r="K9" s="12">
-        <v>5</v>
-      </c>
-      <c r="L9" t="s">
-        <v>83</v>
-      </c>
-      <c r="M9">
-        <v>121</v>
-      </c>
-      <c r="N9">
-        <v>53</v>
-      </c>
-      <c r="O9">
-        <v>77</v>
-      </c>
-      <c r="P9">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:8" ht="39" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -1158,809 +1035,463 @@
         <v>36</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G10" s="3"/>
       <c r="H10" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="J10" s="13"/>
-      <c r="K10" s="12">
-        <v>6</v>
-      </c>
-      <c r="L10" t="s">
-        <v>83</v>
-      </c>
-      <c r="M10">
-        <v>122</v>
-      </c>
-      <c r="N10">
-        <v>54</v>
-      </c>
-      <c r="O10">
-        <v>78</v>
-      </c>
-      <c r="P10">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="39" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>10</v>
       </c>
       <c r="B11" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C11" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="D11" s="3" t="s">
         <v>39</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>40</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>16</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G11" s="3"/>
       <c r="H11" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="J11" s="13"/>
-      <c r="K11" s="12">
-        <v>7</v>
-      </c>
-      <c r="L11" t="s">
-        <v>83</v>
-      </c>
-      <c r="M11">
-        <v>123</v>
-      </c>
-      <c r="N11">
-        <v>55</v>
-      </c>
-      <c r="O11">
-        <v>79</v>
-      </c>
-      <c r="P11">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="12" spans="1:8" ht="39" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>11</v>
       </c>
       <c r="B12" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C12" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="C12" s="3" t="s">
-        <v>42</v>
-      </c>
       <c r="D12" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E12" s="3" t="s">
         <v>16</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G12" s="3"/>
       <c r="H12" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="J12" s="13"/>
-      <c r="K12" s="12">
-        <v>8</v>
-      </c>
-      <c r="L12" t="s">
-        <v>83</v>
-      </c>
-      <c r="M12">
-        <v>124</v>
-      </c>
-      <c r="N12">
-        <v>56</v>
-      </c>
-      <c r="O12">
-        <v>80</v>
-      </c>
-      <c r="P12">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" ht="64.5" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="13" spans="1:8" ht="64.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>12</v>
       </c>
       <c r="B13" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D13" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="C13" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="D13" s="5" t="s">
+      <c r="E13" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="E13" s="3" t="s">
-        <v>45</v>
-      </c>
       <c r="F13" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G13" s="3"/>
       <c r="H13" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="J13" s="13"/>
-      <c r="K13" s="12">
-        <v>9</v>
-      </c>
-      <c r="L13" t="s">
-        <v>83</v>
-      </c>
-      <c r="M13">
-        <v>125</v>
-      </c>
-      <c r="N13">
-        <v>57</v>
-      </c>
-      <c r="O13">
-        <v>81</v>
-      </c>
-      <c r="P13">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" ht="64.5" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="14" spans="1:8" ht="64.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>13</v>
       </c>
       <c r="B14" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="C14" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="D14" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="D14" s="3" t="s">
-        <v>48</v>
-      </c>
       <c r="E14" s="3" t="s">
         <v>21</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G14" s="3"/>
       <c r="H14" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="J14" s="13"/>
-      <c r="K14" s="12">
-        <v>10</v>
-      </c>
-      <c r="L14" t="s">
-        <v>83</v>
-      </c>
-      <c r="M14">
-        <v>126</v>
-      </c>
-      <c r="N14">
-        <v>58</v>
-      </c>
-      <c r="O14">
-        <v>82</v>
-      </c>
-      <c r="P14">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16" ht="64.5" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="15" spans="1:8" ht="64.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
         <v>14</v>
       </c>
       <c r="B15" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="C15" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="C15" s="3" t="s">
-        <v>50</v>
-      </c>
       <c r="D15" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E15" s="3" t="s">
         <v>21</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G15" s="3"/>
       <c r="H15" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="J15" s="13"/>
-      <c r="K15" s="12">
-        <v>11</v>
-      </c>
-      <c r="L15" t="s">
-        <v>83</v>
-      </c>
-      <c r="M15">
-        <v>127</v>
-      </c>
-      <c r="N15">
-        <v>59</v>
-      </c>
-      <c r="O15">
-        <v>83</v>
-      </c>
-      <c r="P15">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="16" spans="1:8" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
         <v>15</v>
       </c>
       <c r="B16" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C16" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="C16" s="5" t="s">
+      <c r="D16" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="D16" s="3" t="s">
-        <v>53</v>
-      </c>
       <c r="E16" s="3" t="s">
         <v>21</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G16" s="3"/>
       <c r="H16" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="J16" s="13"/>
-      <c r="K16" s="12">
-        <v>12</v>
-      </c>
-      <c r="L16" t="s">
-        <v>83</v>
-      </c>
-      <c r="M16" t="s">
-        <v>83</v>
-      </c>
-      <c r="N16">
-        <v>60</v>
-      </c>
-      <c r="O16">
-        <v>84</v>
-      </c>
-      <c r="P16">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="17" spans="1:16" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="17" spans="1:8" ht="39" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
         <v>16</v>
       </c>
       <c r="B17" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="C17" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="D17" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="D17" s="3" t="s">
-        <v>56</v>
-      </c>
       <c r="E17" s="3" t="s">
         <v>21</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G17" s="3"/>
       <c r="H17" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="J17" s="13"/>
-      <c r="K17" s="12">
-        <v>13</v>
-      </c>
-      <c r="L17" t="s">
-        <v>83</v>
-      </c>
-      <c r="M17" t="s">
-        <v>83</v>
-      </c>
-      <c r="N17">
-        <v>61</v>
-      </c>
-      <c r="O17">
-        <v>85</v>
-      </c>
-      <c r="P17">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="18" spans="1:16" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="18" spans="1:8" ht="39" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
         <v>17</v>
       </c>
       <c r="B18" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="C18" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="C18" s="3" t="s">
-        <v>58</v>
-      </c>
       <c r="D18" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E18" s="3" t="s">
         <v>21</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G18" s="3"/>
       <c r="H18" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="J18" s="14" t="s">
-        <v>89</v>
-      </c>
-      <c r="K18" s="15">
-        <v>0</v>
-      </c>
-      <c r="L18">
-        <v>0</v>
-      </c>
-      <c r="M18">
-        <v>0</v>
-      </c>
-      <c r="N18">
-        <v>62</v>
-      </c>
-      <c r="O18">
-        <v>86</v>
-      </c>
-      <c r="P18">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="19" spans="1:16" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="19" spans="1:8" ht="39" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
         <v>18</v>
       </c>
       <c r="B19" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="C19" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="C19" s="3" t="s">
-        <v>60</v>
-      </c>
       <c r="D19" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E19" s="3" t="s">
         <v>21</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G19" s="3"/>
       <c r="H19" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="J19" s="13"/>
-      <c r="K19" s="15">
-        <v>1</v>
-      </c>
-      <c r="L19">
-        <v>1</v>
-      </c>
-      <c r="M19">
-        <v>1</v>
-      </c>
-      <c r="N19">
-        <v>63</v>
-      </c>
-      <c r="O19">
-        <v>87</v>
-      </c>
-      <c r="P19">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="20" spans="1:16" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="20" spans="1:8" ht="39" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="2">
         <v>19</v>
       </c>
       <c r="B20" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="C20" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="C20" s="3" t="s">
-        <v>62</v>
-      </c>
       <c r="D20" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E20" s="3" t="s">
         <v>21</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G20" s="3"/>
       <c r="H20" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="J20" s="16" t="s">
-        <v>90</v>
-      </c>
-      <c r="K20" s="17">
-        <v>0</v>
-      </c>
-      <c r="L20">
-        <v>0</v>
-      </c>
-      <c r="M20">
-        <v>0</v>
-      </c>
-      <c r="N20">
-        <v>64</v>
-      </c>
-      <c r="O20">
-        <v>88</v>
-      </c>
-      <c r="P20">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="21" spans="1:16" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="21" spans="1:8" ht="39" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="2">
         <v>20</v>
       </c>
       <c r="B21" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="C21" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="C21" s="3" t="s">
-        <v>64</v>
-      </c>
       <c r="D21" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E21" s="3" t="s">
         <v>21</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G21" s="3"/>
       <c r="H21" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="J21" s="13"/>
-      <c r="K21" s="17">
-        <v>1</v>
-      </c>
-      <c r="L21">
-        <v>1</v>
-      </c>
-      <c r="M21">
-        <v>1</v>
-      </c>
-      <c r="N21">
+    </row>
+    <row r="22" spans="1:8" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="2">
+        <v>21</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="C22" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="O21">
-        <v>89</v>
-      </c>
-      <c r="P21">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="22" spans="1:16" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="2">
-        <v>21</v>
-      </c>
-      <c r="B22" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>66</v>
-      </c>
       <c r="D22" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E22" s="3" t="s">
         <v>21</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G22" s="3"/>
       <c r="H22" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="J22" s="13"/>
-      <c r="K22" s="17">
-        <v>2</v>
-      </c>
-      <c r="L22">
-        <v>2</v>
-      </c>
-      <c r="M22">
-        <v>2</v>
-      </c>
-      <c r="N22">
-        <v>66</v>
-      </c>
-      <c r="O22">
-        <v>90</v>
-      </c>
-      <c r="P22">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="23" spans="1:16" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="23" spans="1:8" ht="39" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="2">
         <v>22</v>
       </c>
       <c r="B23" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="C23" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="C23" s="3" t="s">
-        <v>68</v>
-      </c>
       <c r="D23" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E23" s="3" t="s">
         <v>21</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G23" s="3"/>
       <c r="H23" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="J23" s="13"/>
-      <c r="K23" s="17">
-        <v>3</v>
-      </c>
-      <c r="L23">
-        <v>3</v>
-      </c>
-      <c r="M23">
-        <v>3</v>
-      </c>
-      <c r="N23">
-        <v>67</v>
-      </c>
-      <c r="O23">
-        <v>91</v>
-      </c>
-      <c r="P23">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="24" spans="1:16" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="24" spans="1:8" ht="39" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="2">
         <v>23</v>
       </c>
       <c r="B24" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="C24" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="C24" s="3" t="s">
-        <v>70</v>
-      </c>
       <c r="D24" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E24" s="3" t="s">
         <v>21</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G24" s="3"/>
       <c r="H24" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="J24" s="13"/>
-      <c r="K24" s="17">
-        <v>4</v>
-      </c>
-      <c r="L24" t="s">
-        <v>83</v>
-      </c>
-      <c r="M24">
-        <v>4</v>
-      </c>
-      <c r="N24">
-        <v>68</v>
-      </c>
-      <c r="O24">
-        <v>92</v>
-      </c>
-      <c r="P24">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="25" spans="1:16" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="25" spans="1:8" ht="39" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="2">
         <v>24</v>
       </c>
       <c r="B25" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="C25" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="C25" s="3" t="s">
-        <v>72</v>
-      </c>
       <c r="D25" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E25" s="3" t="s">
         <v>21</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G25" s="3"/>
       <c r="H25" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="J25" s="13"/>
-      <c r="K25" s="17">
-        <v>5</v>
-      </c>
-      <c r="L25" t="s">
-        <v>83</v>
-      </c>
-      <c r="M25">
-        <v>5</v>
-      </c>
-      <c r="N25">
-        <v>69</v>
-      </c>
-      <c r="O25">
-        <v>93</v>
-      </c>
-      <c r="P25">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="26" spans="1:16" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="26" spans="1:8" ht="39" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="2">
         <v>25</v>
       </c>
       <c r="B26" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="C26" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="C26" s="3" t="s">
-        <v>74</v>
-      </c>
       <c r="D26" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E26" s="3" t="s">
         <v>21</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G26" s="3"/>
       <c r="H26" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="J26" s="13"/>
-      <c r="K26" s="17">
-        <v>6</v>
-      </c>
-      <c r="L26" t="s">
-        <v>83</v>
-      </c>
-      <c r="M26">
-        <v>6</v>
-      </c>
-      <c r="N26">
-        <v>70</v>
-      </c>
-      <c r="O26">
-        <v>94</v>
-      </c>
-      <c r="P26">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="27" spans="1:16" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="27" spans="1:8" ht="39" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="2">
         <v>26</v>
       </c>
       <c r="B27" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="C27" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="C27" s="3" t="s">
-        <v>76</v>
-      </c>
       <c r="D27" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E27" s="3" t="s">
         <v>21</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G27" s="3"/>
       <c r="H27" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="J27" s="13"/>
-      <c r="K27" s="17">
-        <v>7</v>
-      </c>
-      <c r="L27" t="s">
-        <v>83</v>
-      </c>
-      <c r="M27">
-        <v>7</v>
-      </c>
-      <c r="N27">
-        <v>71</v>
-      </c>
-      <c r="O27">
-        <v>95</v>
-      </c>
-      <c r="P27">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="28" spans="1:16" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="28" spans="1:8" ht="39" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="2">
         <v>27</v>
       </c>
       <c r="B28" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C28" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="C28" s="3" t="s">
-        <v>78</v>
-      </c>
       <c r="D28" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E28" s="3" t="s">
         <v>21</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G28" s="3"/>
       <c r="H28" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="29" spans="1:16" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8" ht="39" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="2">
         <v>28</v>
       </c>
       <c r="B29" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="C29" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="C29" s="3" t="s">
-        <v>80</v>
-      </c>
       <c r="D29" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E29" s="3" t="s">
         <v>21</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G29" s="3"/>
       <c r="H29" s="3" t="s">
@@ -1977,12 +1508,554 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="10"/>
+      <c r="B1" s="10"/>
+      <c r="D1" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="10"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="G2" s="11" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="B3" s="13">
+        <v>0</v>
+      </c>
+      <c r="C3" s="10">
+        <v>0</v>
+      </c>
+      <c r="D3" s="10">
+        <v>0</v>
+      </c>
+      <c r="E3" s="10">
+        <v>48</v>
+      </c>
+      <c r="F3" s="10">
+        <v>72</v>
+      </c>
+      <c r="G3" s="10">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="14"/>
+      <c r="B4" s="13">
+        <v>1</v>
+      </c>
+      <c r="C4" s="10">
+        <v>1</v>
+      </c>
+      <c r="D4" s="10">
+        <v>1</v>
+      </c>
+      <c r="E4" s="10">
+        <v>49</v>
+      </c>
+      <c r="F4" s="10">
+        <v>73</v>
+      </c>
+      <c r="G4" s="10">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="14"/>
+      <c r="B5" s="13">
+        <v>2</v>
+      </c>
+      <c r="C5" s="10">
+        <v>2</v>
+      </c>
+      <c r="D5" s="10">
+        <v>2</v>
+      </c>
+      <c r="E5" s="10">
+        <v>50</v>
+      </c>
+      <c r="F5" s="10">
+        <v>74</v>
+      </c>
+      <c r="G5" s="10">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="14"/>
+      <c r="B6" s="13">
+        <v>3</v>
+      </c>
+      <c r="C6" s="10">
+        <v>3</v>
+      </c>
+      <c r="D6" s="10">
+        <v>3</v>
+      </c>
+      <c r="E6" s="10">
+        <v>51</v>
+      </c>
+      <c r="F6" s="10">
+        <v>75</v>
+      </c>
+      <c r="G6" s="10">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="14"/>
+      <c r="B7" s="13">
+        <v>4</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="D7" s="10">
+        <v>120</v>
+      </c>
+      <c r="E7" s="10">
+        <v>52</v>
+      </c>
+      <c r="F7" s="10">
+        <v>76</v>
+      </c>
+      <c r="G7" s="10">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="14"/>
+      <c r="B8" s="13">
+        <v>5</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="D8" s="10">
+        <v>121</v>
+      </c>
+      <c r="E8" s="10">
+        <v>53</v>
+      </c>
+      <c r="F8" s="10">
+        <v>77</v>
+      </c>
+      <c r="G8" s="10">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="14"/>
+      <c r="B9" s="13">
+        <v>6</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="D9" s="10">
+        <v>122</v>
+      </c>
+      <c r="E9" s="10">
+        <v>54</v>
+      </c>
+      <c r="F9" s="10">
+        <v>78</v>
+      </c>
+      <c r="G9" s="10">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="14"/>
+      <c r="B10" s="13">
+        <v>7</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="D10" s="10">
+        <v>123</v>
+      </c>
+      <c r="E10" s="10">
+        <v>55</v>
+      </c>
+      <c r="F10" s="10">
+        <v>79</v>
+      </c>
+      <c r="G10" s="10">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="14"/>
+      <c r="B11" s="13">
+        <v>8</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="D11" s="10">
+        <v>124</v>
+      </c>
+      <c r="E11" s="10">
+        <v>56</v>
+      </c>
+      <c r="F11" s="10">
+        <v>80</v>
+      </c>
+      <c r="G11" s="10">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="14"/>
+      <c r="B12" s="13">
+        <v>9</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="D12" s="10">
+        <v>125</v>
+      </c>
+      <c r="E12" s="10">
+        <v>57</v>
+      </c>
+      <c r="F12" s="10">
+        <v>81</v>
+      </c>
+      <c r="G12" s="10">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="14"/>
+      <c r="B13" s="13">
+        <v>10</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="D13" s="10">
+        <v>126</v>
+      </c>
+      <c r="E13" s="10">
+        <v>58</v>
+      </c>
+      <c r="F13" s="10">
+        <v>82</v>
+      </c>
+      <c r="G13" s="10">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="14"/>
+      <c r="B14" s="13">
+        <v>11</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="D14" s="10">
+        <v>127</v>
+      </c>
+      <c r="E14" s="10">
+        <v>59</v>
+      </c>
+      <c r="F14" s="10">
+        <v>83</v>
+      </c>
+      <c r="G14" s="10">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="14"/>
+      <c r="B15" s="13">
+        <v>12</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="D15" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="E15" s="10">
+        <v>60</v>
+      </c>
+      <c r="F15" s="10">
+        <v>84</v>
+      </c>
+      <c r="G15" s="10">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="14"/>
+      <c r="B16" s="13">
+        <v>13</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="D16" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="E16" s="10">
+        <v>61</v>
+      </c>
+      <c r="F16" s="10">
+        <v>85</v>
+      </c>
+      <c r="G16" s="10">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="B17" s="16">
+        <v>0</v>
+      </c>
+      <c r="C17" s="10">
+        <v>0</v>
+      </c>
+      <c r="D17" s="10">
+        <v>0</v>
+      </c>
+      <c r="E17" s="10">
+        <v>62</v>
+      </c>
+      <c r="F17" s="10">
+        <v>86</v>
+      </c>
+      <c r="G17" s="10">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="14"/>
+      <c r="B18" s="16">
+        <v>1</v>
+      </c>
+      <c r="C18" s="10">
+        <v>1</v>
+      </c>
+      <c r="D18" s="10">
+        <v>1</v>
+      </c>
+      <c r="E18" s="10">
+        <v>63</v>
+      </c>
+      <c r="F18" s="10">
+        <v>87</v>
+      </c>
+      <c r="G18" s="10">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="B19" s="18">
+        <v>0</v>
+      </c>
+      <c r="C19" s="10">
+        <v>0</v>
+      </c>
+      <c r="D19" s="10">
+        <v>0</v>
+      </c>
+      <c r="E19" s="10">
+        <v>64</v>
+      </c>
+      <c r="F19" s="10">
+        <v>88</v>
+      </c>
+      <c r="G19" s="10">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="14"/>
+      <c r="B20" s="18">
+        <v>1</v>
+      </c>
+      <c r="C20" s="10">
+        <v>1</v>
+      </c>
+      <c r="D20" s="10">
+        <v>1</v>
+      </c>
+      <c r="E20" s="10">
+        <v>65</v>
+      </c>
+      <c r="F20" s="10">
+        <v>89</v>
+      </c>
+      <c r="G20" s="10">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="14"/>
+      <c r="B21" s="18">
+        <v>2</v>
+      </c>
+      <c r="C21" s="10">
+        <v>2</v>
+      </c>
+      <c r="D21" s="10">
+        <v>2</v>
+      </c>
+      <c r="E21" s="10">
+        <v>66</v>
+      </c>
+      <c r="F21" s="10">
+        <v>90</v>
+      </c>
+      <c r="G21" s="10">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="14"/>
+      <c r="B22" s="18">
+        <v>3</v>
+      </c>
+      <c r="C22" s="10">
+        <v>3</v>
+      </c>
+      <c r="D22" s="10">
+        <v>3</v>
+      </c>
+      <c r="E22" s="10">
+        <v>67</v>
+      </c>
+      <c r="F22" s="10">
+        <v>91</v>
+      </c>
+      <c r="G22" s="10">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="14"/>
+      <c r="B23" s="18">
+        <v>4</v>
+      </c>
+      <c r="C23" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="D23" s="10">
+        <v>4</v>
+      </c>
+      <c r="E23" s="10">
+        <v>68</v>
+      </c>
+      <c r="F23" s="10">
+        <v>92</v>
+      </c>
+      <c r="G23" s="10">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="14"/>
+      <c r="B24" s="18">
+        <v>5</v>
+      </c>
+      <c r="C24" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="D24" s="10">
+        <v>5</v>
+      </c>
+      <c r="E24" s="10">
+        <v>69</v>
+      </c>
+      <c r="F24" s="10">
+        <v>93</v>
+      </c>
+      <c r="G24" s="10">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="14"/>
+      <c r="B25" s="18">
+        <v>6</v>
+      </c>
+      <c r="C25" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="D25" s="10">
+        <v>6</v>
+      </c>
+      <c r="E25" s="10">
+        <v>70</v>
+      </c>
+      <c r="F25" s="10">
+        <v>94</v>
+      </c>
+      <c r="G25" s="10">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="14"/>
+      <c r="B26" s="18">
+        <v>7</v>
+      </c>
+      <c r="C26" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="D26" s="10">
+        <v>7</v>
+      </c>
+      <c r="E26" s="10">
+        <v>71</v>
+      </c>
+      <c r="F26" s="10">
+        <v>95</v>
+      </c>
+      <c r="G26" s="10">
+        <v>119</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
added thermistor Omega 44044 formula
</commit_message>
<xml_diff>
--- a/LJDAQChannelGuide.xlsx
+++ b/LJDAQChannelGuide.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="172">
   <si>
     <t>i</t>
   </si>
@@ -282,10 +282,6 @@
     <t>FIO# on Board</t>
   </si>
   <si>
-    <t xml:space="preserve">Positive:
-Negative: </t>
-  </si>
-  <si>
     <t>Board Number</t>
   </si>
   <si>
@@ -317,13 +313,263 @@
   </si>
   <si>
     <t>On Labjack</t>
+  </si>
+  <si>
+    <t>Differential Blocks</t>
+  </si>
+  <si>
+    <t>P Channel</t>
+  </si>
+  <si>
+    <t>N Channel</t>
+  </si>
+  <si>
+    <t>Connector</t>
+  </si>
+  <si>
+    <t>Block 1</t>
+  </si>
+  <si>
+    <t>M48-55</t>
+  </si>
+  <si>
+    <t>M56-63</t>
+  </si>
+  <si>
+    <t>Block 2</t>
+  </si>
+  <si>
+    <t>M64-71</t>
+  </si>
+  <si>
+    <t>M72-79</t>
+  </si>
+  <si>
+    <t>X3 &amp; X4</t>
+  </si>
+  <si>
+    <t>Block 3</t>
+  </si>
+  <si>
+    <t>M80-87</t>
+  </si>
+  <si>
+    <t>M88-95</t>
+  </si>
+  <si>
+    <t>Block 4</t>
+  </si>
+  <si>
+    <t>M96-103</t>
+  </si>
+  <si>
+    <t>M104-111</t>
+  </si>
+  <si>
+    <t>Block 5</t>
+  </si>
+  <si>
+    <t>M112-119</t>
+  </si>
+  <si>
+    <t>M120-127</t>
+  </si>
+  <si>
+    <t>X5 &amp; X2</t>
+  </si>
+  <si>
+    <t>Positive: X3, AIN0
+Negative: X3, AIN8</t>
+  </si>
+  <si>
+    <t>Positive: X3, AIN1
+Negative: X3, AIN9</t>
+  </si>
+  <si>
+    <t>Positive: X3, AIN2
+Negative: X3, AIN10</t>
+  </si>
+  <si>
+    <t>Positive: X3, AIN3
+Negative: X3, AIN11</t>
+  </si>
+  <si>
+    <t>48/56</t>
+  </si>
+  <si>
+    <t>49/57</t>
+  </si>
+  <si>
+    <t>50/58</t>
+  </si>
+  <si>
+    <t>51/59</t>
+  </si>
+  <si>
+    <t>52/60</t>
+  </si>
+  <si>
+    <t>Positive: X3, AIN4
+Negative: X3, AIN12</t>
+  </si>
+  <si>
+    <t>53/61</t>
+  </si>
+  <si>
+    <t>Positive: X3, AIN5
+Negative: X3, AIN13</t>
+  </si>
+  <si>
+    <t>Positive: X3, AIN6
+Negative: X3, DAC0</t>
+  </si>
+  <si>
+    <t>54/62</t>
+  </si>
+  <si>
+    <t>Positive: X3, AIN7
+Negative: X3, DAC1</t>
+  </si>
+  <si>
+    <t>55/63</t>
+  </si>
+  <si>
+    <t>80/88</t>
+  </si>
+  <si>
+    <t>Positive: X4, AIN8
+Negative: X4, FIO0</t>
+  </si>
+  <si>
+    <t>81/89</t>
+  </si>
+  <si>
+    <t>Positive: X4, AIN9
+Negative: X4, FIO1</t>
+  </si>
+  <si>
+    <t>82/90</t>
+  </si>
+  <si>
+    <t>Positive: X4, AIN10
+Negative: X4, FIO2</t>
+  </si>
+  <si>
+    <t>Positive: X4, AIN11
+Negative: X4, FIO3</t>
+  </si>
+  <si>
+    <t>83/91</t>
+  </si>
+  <si>
+    <t>Positive: X4, AIN12
+Negative: X4, FIO4</t>
+  </si>
+  <si>
+    <t>84/92</t>
+  </si>
+  <si>
+    <t>Positive: X4, AIN13
+Negative: X4, FIO5</t>
+  </si>
+  <si>
+    <t>85/93</t>
+  </si>
+  <si>
+    <t>Positive: X4, DAC0
+Negative: X4, FIO6</t>
+  </si>
+  <si>
+    <t>86/94</t>
+  </si>
+  <si>
+    <t>Positive: X4, DAC1
+Negative: X4, FIO7</t>
+  </si>
+  <si>
+    <t>87/95</t>
+  </si>
+  <si>
+    <t>Positive: X5, AIN0
+Negative: X5, AIN8</t>
+  </si>
+  <si>
+    <t>96/104</t>
+  </si>
+  <si>
+    <t>Positive: X5, AIN1
+Negative: X5, AIN9</t>
+  </si>
+  <si>
+    <t>97/105</t>
+  </si>
+  <si>
+    <t>Positive: X5, AIN2
+Negative: X5, AIN10</t>
+  </si>
+  <si>
+    <t>98/106</t>
+  </si>
+  <si>
+    <t>Positive: X5, AIN3
+Negative: X5, AIN11</t>
+  </si>
+  <si>
+    <t>99/107</t>
+  </si>
+  <si>
+    <t>Positive: X5, AIN4
+Negative: X5, AIN12</t>
+  </si>
+  <si>
+    <t>100/108</t>
+  </si>
+  <si>
+    <t>Positive: X5, AIN5
+Negative: X5, AIN13</t>
+  </si>
+  <si>
+    <t>101/109</t>
+  </si>
+  <si>
+    <t>Positive: X5, AIN6
+Negative: X5, DAC0</t>
+  </si>
+  <si>
+    <t>102/110</t>
+  </si>
+  <si>
+    <t>Used</t>
+  </si>
+  <si>
+    <t>Used up to 102/110</t>
+  </si>
+  <si>
+    <t>Positive: X2, AIN4
+Negative: GND</t>
+  </si>
+  <si>
+    <t>Positive: X2, AIN5
+Negative: GND</t>
+  </si>
+  <si>
+    <t>Positive: X2, AIN6
+Negative: GND</t>
+  </si>
+  <si>
+    <t>Positive: X2, AIN7
+Negative: GND</t>
+  </si>
+  <si>
+    <t>Positive: X2, AIN8
+Negative: GND</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -360,8 +606,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="13">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -434,8 +693,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -469,12 +734,43 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
@@ -541,6 +837,18 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -846,8 +1154,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2:G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -881,16 +1189,16 @@
         <v>6</v>
       </c>
       <c r="H1" s="19" t="s">
+        <v>90</v>
+      </c>
+      <c r="I1" s="20" t="s">
+        <v>89</v>
+      </c>
+      <c r="J1" s="20" t="s">
+        <v>88</v>
+      </c>
+      <c r="K1" s="21" t="s">
         <v>91</v>
-      </c>
-      <c r="I1" s="20" t="s">
-        <v>90</v>
-      </c>
-      <c r="J1" s="20" t="s">
-        <v>89</v>
-      </c>
-      <c r="K1" s="21" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="39" thickBot="1" x14ac:dyDescent="0.3">
@@ -910,14 +1218,16 @@
         <v>10</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="G2" s="2"/>
+        <v>119</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>123</v>
+      </c>
       <c r="H2" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="I2" s="18" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="K2" t="b">
         <v>0</v>
@@ -940,14 +1250,16 @@
         <v>14</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="G3" s="2"/>
+        <v>167</v>
+      </c>
+      <c r="G3" s="2">
+        <v>120</v>
+      </c>
       <c r="H3" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="I3" s="18" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="K3" t="b">
         <v>0</v>
@@ -970,14 +1282,16 @@
         <v>18</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="G4" s="2"/>
+        <v>120</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>124</v>
+      </c>
       <c r="H4" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="I4" s="18" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J4">
         <v>2</v>
@@ -1003,14 +1317,16 @@
         <v>18</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="G5" s="2"/>
+        <v>121</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>125</v>
+      </c>
       <c r="H5" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="I5" s="18" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J5">
         <v>2</v>
@@ -1036,14 +1352,16 @@
         <v>18</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="G6" s="2"/>
+        <v>122</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>126</v>
+      </c>
       <c r="H6" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="I6" s="18" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J6">
         <v>2</v>
@@ -1069,14 +1387,16 @@
         <v>18</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="G7" s="2"/>
+        <v>128</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>127</v>
+      </c>
       <c r="H7" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="I7" s="18" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J7">
         <v>2</v>
@@ -1102,14 +1422,16 @@
         <v>18</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="G8" s="2"/>
+        <v>130</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>129</v>
+      </c>
       <c r="H8" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="I8" s="18" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J8">
         <v>2</v>
@@ -1135,14 +1457,16 @@
         <v>18</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="G9" s="2"/>
+        <v>131</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>132</v>
+      </c>
       <c r="H9" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="I9" s="18" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J9">
         <v>2</v>
@@ -1168,14 +1492,16 @@
         <v>33</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="G10" s="2"/>
+        <v>168</v>
+      </c>
+      <c r="G10" s="2">
+        <v>121</v>
+      </c>
       <c r="H10" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I10" s="18" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="K10" t="b">
         <v>0</v>
@@ -1198,14 +1524,16 @@
         <v>14</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="G11" s="2"/>
+        <v>169</v>
+      </c>
+      <c r="G11" s="2">
+        <v>122</v>
+      </c>
       <c r="H11" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="I11" s="18" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="K11" t="b">
         <v>0</v>
@@ -1228,14 +1556,16 @@
         <v>14</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="G12" s="2"/>
+        <v>170</v>
+      </c>
+      <c r="G12" s="2">
+        <v>123</v>
+      </c>
       <c r="H12" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="I12" s="18" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="K12" t="b">
         <v>0</v>
@@ -1258,14 +1588,16 @@
         <v>41</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="G13" s="2"/>
+        <v>171</v>
+      </c>
+      <c r="G13" s="2">
+        <v>124</v>
+      </c>
       <c r="H13" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="I13" s="18" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="K13" t="b">
         <v>0</v>
@@ -1288,14 +1620,16 @@
         <v>18</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="G14" s="2"/>
+        <v>133</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>134</v>
+      </c>
       <c r="H14" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="I14" s="18" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J14">
         <v>2</v>
@@ -1321,14 +1655,16 @@
         <v>18</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="G15" s="2"/>
+        <v>136</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>135</v>
+      </c>
       <c r="H15" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="I15" s="18" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J15">
         <v>2</v>
@@ -1354,14 +1690,16 @@
         <v>18</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="G16" s="2"/>
+        <v>138</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>137</v>
+      </c>
       <c r="H16" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="I16" s="18" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J16">
         <v>2</v>
@@ -1387,14 +1725,16 @@
         <v>18</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="G17" s="2"/>
+        <v>140</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>139</v>
+      </c>
       <c r="H17" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="I17" s="18" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J17">
         <v>2</v>
@@ -1420,14 +1760,16 @@
         <v>18</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="G18" s="2"/>
+        <v>141</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>142</v>
+      </c>
       <c r="H18" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="I18" s="18" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J18">
         <v>2</v>
@@ -1453,14 +1795,16 @@
         <v>18</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="G19" s="2"/>
+        <v>143</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>144</v>
+      </c>
       <c r="H19" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="I19" s="18" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J19">
         <v>2</v>
@@ -1486,14 +1830,16 @@
         <v>18</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="G20" s="2"/>
+        <v>145</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>146</v>
+      </c>
       <c r="H20" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="I20" s="18" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J20">
         <v>2</v>
@@ -1519,14 +1865,16 @@
         <v>18</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="G21" s="2"/>
+        <v>147</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>148</v>
+      </c>
       <c r="H21" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="I21" s="18" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J21">
         <v>2</v>
@@ -1552,14 +1900,16 @@
         <v>18</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="G22" s="2"/>
+        <v>149</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>150</v>
+      </c>
       <c r="H22" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="I22" s="18" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J22">
         <v>2</v>
@@ -1585,14 +1935,16 @@
         <v>18</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="G23" s="2"/>
+        <v>151</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>152</v>
+      </c>
       <c r="H23" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="I23" s="18" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J23">
         <v>2</v>
@@ -1618,14 +1970,16 @@
         <v>18</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="G24" s="2"/>
+        <v>153</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>154</v>
+      </c>
       <c r="H24" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="I24" s="18" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J24">
         <v>2</v>
@@ -1651,14 +2005,16 @@
         <v>18</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="G25" s="2"/>
+        <v>155</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>156</v>
+      </c>
       <c r="H25" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="I25" s="18" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J25">
         <v>2</v>
@@ -1684,14 +2040,16 @@
         <v>18</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="G26" s="2"/>
+        <v>157</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>158</v>
+      </c>
       <c r="H26" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="I26" s="18" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J26">
         <v>2</v>
@@ -1717,14 +2075,16 @@
         <v>18</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="G27" s="2"/>
+        <v>159</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>160</v>
+      </c>
       <c r="H27" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="I27" s="18" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J27">
         <v>2</v>
@@ -1750,14 +2110,16 @@
         <v>18</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="G28" s="2"/>
+        <v>161</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>162</v>
+      </c>
       <c r="H28" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="I28" s="18" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J28">
         <v>2</v>
@@ -1783,14 +2145,16 @@
         <v>18</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="G29" s="2"/>
+        <v>163</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>164</v>
+      </c>
       <c r="H29" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="I29" s="18" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J29">
         <v>2</v>
@@ -1804,10 +2168,10 @@
         <v>29</v>
       </c>
       <c r="B30" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="C30" s="18" t="s">
         <v>97</v>
-      </c>
-      <c r="C30" s="18" t="s">
-        <v>98</v>
       </c>
       <c r="D30" s="18" t="s">
         <v>18</v>
@@ -1822,10 +2186,10 @@
         <v>14</v>
       </c>
       <c r="H30" s="18" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="I30" s="18" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="J30">
         <v>0</v>
@@ -1845,15 +2209,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H26"/>
+  <dimension ref="A1:N26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="9"/>
       <c r="B1" s="9"/>
       <c r="D1" s="9" t="s">
@@ -1863,7 +2227,7 @@
       <c r="F1" s="9"/>
       <c r="G1" s="9"/>
     </row>
-    <row r="2" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="9"/>
       <c r="B2" s="9"/>
       <c r="C2" s="17" t="s">
@@ -1882,10 +2246,10 @@
         <v>84</v>
       </c>
       <c r="H2" s="17" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
         <v>80</v>
       </c>
@@ -1908,7 +2272,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="12"/>
       <c r="B4" s="11">
         <v>1</v>
@@ -1928,8 +2292,20 @@
       <c r="G4" s="9">
         <v>97</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J4" s="23" t="s">
+        <v>98</v>
+      </c>
+      <c r="K4" s="23" t="s">
+        <v>99</v>
+      </c>
+      <c r="L4" s="23" t="s">
+        <v>100</v>
+      </c>
+      <c r="M4" s="23" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="12"/>
       <c r="B5" s="11">
         <v>2</v>
@@ -1949,8 +2325,23 @@
       <c r="G5" s="9">
         <v>98</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J5" s="24" t="s">
+        <v>102</v>
+      </c>
+      <c r="K5" s="24" t="s">
+        <v>103</v>
+      </c>
+      <c r="L5" s="24" t="s">
+        <v>104</v>
+      </c>
+      <c r="M5" s="25" t="s">
+        <v>82</v>
+      </c>
+      <c r="N5" s="26" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="12"/>
       <c r="B6" s="11">
         <v>3</v>
@@ -1970,8 +2361,20 @@
       <c r="G6" s="9">
         <v>99</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J6" s="24" t="s">
+        <v>105</v>
+      </c>
+      <c r="K6" s="24" t="s">
+        <v>106</v>
+      </c>
+      <c r="L6" s="24" t="s">
+        <v>107</v>
+      </c>
+      <c r="M6" s="25" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="12"/>
       <c r="B7" s="11">
         <v>4</v>
@@ -1991,8 +2394,23 @@
       <c r="G7" s="9">
         <v>100</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J7" s="24" t="s">
+        <v>109</v>
+      </c>
+      <c r="K7" s="24" t="s">
+        <v>110</v>
+      </c>
+      <c r="L7" s="24" t="s">
+        <v>111</v>
+      </c>
+      <c r="M7" s="25" t="s">
+        <v>83</v>
+      </c>
+      <c r="N7" s="26" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="12"/>
       <c r="B8" s="11">
         <v>5</v>
@@ -2012,8 +2430,23 @@
       <c r="G8" s="9">
         <v>101</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J8" s="24" t="s">
+        <v>112</v>
+      </c>
+      <c r="K8" s="24" t="s">
+        <v>113</v>
+      </c>
+      <c r="L8" s="24" t="s">
+        <v>114</v>
+      </c>
+      <c r="M8" s="25" t="s">
+        <v>84</v>
+      </c>
+      <c r="N8" s="26" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="12"/>
       <c r="B9" s="11">
         <v>6</v>
@@ -2033,8 +2466,20 @@
       <c r="G9" s="9">
         <v>102</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J9" s="24" t="s">
+        <v>115</v>
+      </c>
+      <c r="K9" s="24" t="s">
+        <v>116</v>
+      </c>
+      <c r="L9" s="24" t="s">
+        <v>117</v>
+      </c>
+      <c r="M9" s="25" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="12"/>
       <c r="B10" s="11">
         <v>7</v>
@@ -2055,7 +2500,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="12"/>
       <c r="B11" s="11">
         <v>8</v>
@@ -2076,7 +2521,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="12"/>
       <c r="B12" s="11">
         <v>9</v>
@@ -2097,7 +2542,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="12"/>
       <c r="B13" s="11">
         <v>10</v>
@@ -2118,7 +2563,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="12"/>
       <c r="B14" s="11">
         <v>11</v>
@@ -2139,7 +2584,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="12"/>
       <c r="B15" s="11">
         <v>12</v>
@@ -2160,7 +2605,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="12"/>
       <c r="B16" s="11">
         <v>13</v>

</xml_diff>